<commit_message>
bug fixes + test ready code added
</commit_message>
<xml_diff>
--- a/MFL-main/mfldir/MFL_Flow_Calibration.xlsx
+++ b/MFL-main/mfldir/MFL_Flow_Calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/MFL-Controls/MFL-main/mfldir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C437BE-7442-CB44-B3F2-EA795671C1E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4410EC77-7979-BB4A-A726-B1E63F04CFE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{1BDBBDA9-319F-5E48-997F-F1AFCC9C0E6B}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{1BDBBDA9-319F-5E48-997F-F1AFCC9C0E6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,7 +385,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,7 +411,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -419,7 +419,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -427,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -435,7 +435,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>80</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -443,7 +443,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -451,7 +451,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>120</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -459,7 +459,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>140</v>
+        <v>50.4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -467,7 +467,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>160</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -475,7 +475,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>180</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -483,7 +483,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>200</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -491,7 +491,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>220</v>
+        <v>79.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -499,7 +499,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>240</v>
+        <v>86.4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -507,7 +507,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>260</v>
+        <v>93.6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -515,7 +515,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>280</v>
+        <v>100.8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -523,7 +523,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>300</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -531,7 +531,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>320</v>
+        <v>115.2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -539,7 +539,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>340</v>
+        <v>122.4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>360</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -555,7 +555,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>380</v>
+        <v>136.80000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>400</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -571,7 +571,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>420</v>
+        <v>151.19999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -579,7 +579,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>440</v>
+        <v>158.4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>460</v>
+        <v>165.6</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>480</v>
+        <v>172.8</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>500</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored dir and removed duplicates
</commit_message>
<xml_diff>
--- a/MFL-main/mfldir/MFL_Flow_Calibration.xlsx
+++ b/MFL-main/mfldir/MFL_Flow_Calibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/MFL-Controls/MFL-main/mfldir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CPcom\Downloads\MFL-Controls-main\MFL-Controls-main\MFL-main\mfldir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4410EC77-7979-BB4A-A726-B1E63F04CFE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABA3565-F69F-407F-A333-53FE853769E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{1BDBBDA9-319F-5E48-997F-F1AFCC9C0E6B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{1BDBBDA9-319F-5E48-997F-F1AFCC9C0E6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0366E6A8-33D0-F249-B65B-03090EC8234D}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,7 +398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -406,7 +406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -414,7 +414,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -422,7 +422,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -430,7 +430,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -438,7 +438,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -446,7 +446,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -454,7 +454,7 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -462,7 +462,7 @@
         <v>50.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -470,7 +470,7 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -478,7 +478,7 @@
         <v>64.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>10</v>
       </c>
@@ -486,7 +486,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>11</v>
       </c>
@@ -494,7 +494,7 @@
         <v>79.2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>12</v>
       </c>
@@ -502,7 +502,7 @@
         <v>86.4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>13</v>
       </c>
@@ -510,7 +510,7 @@
         <v>93.6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>14</v>
       </c>
@@ -518,7 +518,7 @@
         <v>100.8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>15</v>
       </c>
@@ -526,7 +526,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>16</v>
       </c>
@@ -534,7 +534,7 @@
         <v>115.2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>17</v>
       </c>
@@ -542,7 +542,7 @@
         <v>122.4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>18</v>
       </c>
@@ -550,7 +550,7 @@
         <v>129.6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>19</v>
       </c>
@@ -558,7 +558,7 @@
         <v>136.80000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>20</v>
       </c>
@@ -566,7 +566,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>21</v>
       </c>
@@ -574,7 +574,7 @@
         <v>151.19999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>22</v>
       </c>
@@ -582,7 +582,7 @@
         <v>158.4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>23</v>
       </c>
@@ -590,7 +590,7 @@
         <v>165.6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>24</v>
       </c>
@@ -598,12 +598,1412 @@
         <v>172.8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
         <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>187.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>194.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>201.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>208.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>223.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>230.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>237.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>244.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>259.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>266.39999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>273.60000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>280.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>295.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>302.39999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>309.60000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>316.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>331.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>338.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>345.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>352.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>367.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>374.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>381.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>388.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>403.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>410.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>417.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>424.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>439.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>446.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>453.6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>460.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>475.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>482.4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>489.6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>496.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>511.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>518.4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>525.6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>532.79999999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>547.20000000000005</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>554.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>561.6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>568.79999999999995</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>583.20000000000005</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>590.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>597.6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>604.79999999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>619.20000000000005</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>626.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>633.6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>640.79999999999995</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>655.20000000000005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>662.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>669.6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>676.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>691.2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>698.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>705.6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>712.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>727.2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>734.4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>741.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>748.8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>763.2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>770.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>777.6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>784.8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>799.2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>806.4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>813.6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>820.8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>835.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>842.4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>849.6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>856.8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>871.2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <v>878.4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>885.6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>892.8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>907.2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>914.4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>921.6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>928.8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>943.2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>950.4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>957.6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>964.8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A137">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A138">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>979.2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A139">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>986.4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A140">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>993.6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A141">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>1000.8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A142">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A143">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>1015.2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A144">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>1022.4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A145">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>1029.5999999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A146">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>1036.8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A147">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A148">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>1051.2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A149">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>1058.4000000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A150">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>1065.5999999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>1072.8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A152">
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A153">
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <v>1087.2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A154">
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <v>1094.4000000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A155">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>1101.5999999999999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A156">
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <v>1108.8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A157">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A158">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>1123.2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A159">
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <v>1130.4000000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A160">
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <v>1137.5999999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A161">
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <v>1144.8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A162">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A163">
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <v>1159.2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A164">
+        <v>162</v>
+      </c>
+      <c r="B164">
+        <v>1166.4000000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A165">
+        <v>163</v>
+      </c>
+      <c r="B165">
+        <v>1173.5999999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A166">
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <v>1180.8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A167">
+        <v>165</v>
+      </c>
+      <c r="B167">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A168">
+        <v>166</v>
+      </c>
+      <c r="B168">
+        <v>1195.2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A169">
+        <v>167</v>
+      </c>
+      <c r="B169">
+        <v>1202.4000000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A170">
+        <v>168</v>
+      </c>
+      <c r="B170">
+        <v>1209.5999999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A171">
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <v>1216.8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A172">
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A173">
+        <v>171</v>
+      </c>
+      <c r="B173">
+        <v>1231.2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A174">
+        <v>172</v>
+      </c>
+      <c r="B174">
+        <v>1238.4000000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A175">
+        <v>173</v>
+      </c>
+      <c r="B175">
+        <v>1245.5999999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A176">
+        <v>174</v>
+      </c>
+      <c r="B176">
+        <v>1252.8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A177">
+        <v>175</v>
+      </c>
+      <c r="B177">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A178">
+        <v>176</v>
+      </c>
+      <c r="B178">
+        <v>1267.2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A179">
+        <v>177</v>
+      </c>
+      <c r="B179">
+        <v>1274.4000000000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A180">
+        <v>178</v>
+      </c>
+      <c r="B180">
+        <v>1281.5999999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A181">
+        <v>179</v>
+      </c>
+      <c r="B181">
+        <v>1288.8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A182">
+        <v>180</v>
+      </c>
+      <c r="B182">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A183">
+        <v>181</v>
+      </c>
+      <c r="B183">
+        <v>1303.2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A184">
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <v>1310.4000000000001</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A185">
+        <v>183</v>
+      </c>
+      <c r="B185">
+        <v>1317.6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A186">
+        <v>184</v>
+      </c>
+      <c r="B186">
+        <v>1324.8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A187">
+        <v>185</v>
+      </c>
+      <c r="B187">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A188">
+        <v>186</v>
+      </c>
+      <c r="B188">
+        <v>1339.2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A189">
+        <v>187</v>
+      </c>
+      <c r="B189">
+        <v>1346.4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A190">
+        <v>188</v>
+      </c>
+      <c r="B190">
+        <v>1353.6</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A191">
+        <v>189</v>
+      </c>
+      <c r="B191">
+        <v>1360.8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A192">
+        <v>190</v>
+      </c>
+      <c r="B192">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A193">
+        <v>191</v>
+      </c>
+      <c r="B193">
+        <v>1375.2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A194">
+        <v>192</v>
+      </c>
+      <c r="B194">
+        <v>1382.4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A195">
+        <v>193</v>
+      </c>
+      <c r="B195">
+        <v>1389.6</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A196">
+        <v>194</v>
+      </c>
+      <c r="B196">
+        <v>1396.8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A197">
+        <v>195</v>
+      </c>
+      <c r="B197">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A198">
+        <v>196</v>
+      </c>
+      <c r="B198">
+        <v>1411.2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A199">
+        <v>197</v>
+      </c>
+      <c r="B199">
+        <v>1418.4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A200">
+        <v>198</v>
+      </c>
+      <c r="B200">
+        <v>1425.6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A201">
+        <v>199</v>
+      </c>
+      <c r="B201">
+        <v>1432.8</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A202">
+        <v>200</v>
+      </c>
+      <c r="B202">
+        <v>1440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>